<commit_message>
figures for paper and analysis cleaned
</commit_message>
<xml_diff>
--- a/GeocodingProfileVsTweet.xlsx
+++ b/GeocodingProfileVsTweet.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Total Tweet Count</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">PLT </t>
   </si>
@@ -35,13 +32,22 @@
     <t>TLT</t>
   </si>
   <si>
-    <t>TLT no PLT</t>
+    <t>Week Beginning on</t>
+  </si>
+  <si>
+    <t>Twitter Tagging Only</t>
+  </si>
+  <si>
+    <t>Profile Tagging Ony</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -73,7 +79,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,12 +131,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>PLT vs</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> TLT (X vs Y)</a:t>
+              <a:t>Weekly Counts of Profile vs. Tweet Geo-Tagging</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -172,8 +174,64 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Fit</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000">
+                  <a:alpha val="33000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Sheet1!$G$2,Sheet1!$G$3)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>350000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Sheet1!$G$2,Sheet1!$G$3)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>350000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Geo</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -196,6 +254,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.1930398776041465E-3"/>
+                  <c:y val="0.17971791176779828"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$55</c:f>
@@ -548,30 +657,73 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="487790984"/>
-        <c:axId val="487790592"/>
+        <c:axId val="466811584"/>
+        <c:axId val="472013504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="487790984"/>
+        <c:axId val="466811584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Profile Geo-Tagging</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -609,14 +761,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487790592"/>
+        <c:crossAx val="472013504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="487790592"/>
+        <c:axId val="472013504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -634,6 +787,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Individual</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Tweet Geo-Tagging</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -671,7 +885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487790984"/>
+        <c:crossAx val="466811584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -683,6 +897,1062 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Volume o</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>f Tweets Geo-Tagged with Only One Method</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19583876802344385"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Profile Tagging Ony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy;@</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>41644</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41651</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41665</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41672</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41679</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41686</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41693</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41707</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41714</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41735</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41742</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41749</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41756</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41763</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41770</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41777</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41784</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41791</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41798</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41805</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41812</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41819</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41826</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41833</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41840</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41847</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41854</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41861</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41868</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41882</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41889</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41903</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41910</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41917</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41924</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41931</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41938</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41945</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41952</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>41959</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>41966</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41973</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41980</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41987</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41994</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42008</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>5992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6613</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6156</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6936</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7314</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8171</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7519</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7586</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7822</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8906</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8563</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21361</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23721</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20364</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21243</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22254</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20389</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20587</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20663</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19101</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18015</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20550</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21522</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20479</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20438</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21029</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18409</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17381</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16492</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>18951</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16896</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15298</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15564</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16142</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11429</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14898</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14632</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13229</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12649</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>16374</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15065</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4784</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14830</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>14874</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>13164</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12170</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>9576</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8959</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>9201</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9983</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Twitter Tagging Only</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy;@</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>41644</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41651</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41658</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41665</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41672</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41679</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41686</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41693</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41707</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41714</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41728</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41735</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41742</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41749</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41756</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41763</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41770</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41777</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41784</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41791</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41798</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41805</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41812</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41819</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41826</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41833</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41840</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41847</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41854</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41861</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41868</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41882</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41889</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41903</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41910</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41917</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41924</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41931</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41938</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41945</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>41952</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>41959</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>41966</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>41973</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41980</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41987</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41994</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42008</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>11623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9529</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9448</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9074</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8890</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8959</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9162</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8438</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6181</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="472012720"/>
+        <c:axId val="472013112"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="472012720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy;@" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472013112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="472013112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472012720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.7268910271783503E-2"/>
+          <c:y val="0.23689741907261591"/>
+          <c:w val="0.20946933184385433"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -760,6 +2030,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1276,20 +2586,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>607218</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>16667</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>645318</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1303,6 +3116,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>621505</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1574,34 +3417,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
-        <v>41643.791666666664</v>
+        <v>41644</v>
       </c>
       <c r="B2">
         <v>94073</v>
@@ -1619,10 +3465,14 @@
         <f>D2/B2</f>
         <v>6.3695215417813825E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>41650.791666666664</v>
+        <f>A2+7</f>
+        <v>41651</v>
       </c>
       <c r="B3">
         <v>100720</v>
@@ -1640,10 +3490,14 @@
         <f t="shared" ref="F3:F55" si="0">D3/B3</f>
         <v>6.5657267672756162E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
-        <v>41657.791666666664</v>
+        <f t="shared" ref="A4:A55" si="1">A3+7</f>
+        <v>41658</v>
       </c>
       <c r="B4">
         <v>96179</v>
@@ -1662,9 +3516,10 @@
         <v>6.4005656120358911E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
-        <v>41664.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41665</v>
       </c>
       <c r="B5">
         <v>87839</v>
@@ -1683,9 +3538,10 @@
         <v>6.5312674324616626E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
-        <v>41671.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41672</v>
       </c>
       <c r="B6">
         <v>88913</v>
@@ -1704,9 +3560,10 @@
         <v>7.8008840102122293E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
-        <v>41678.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41679</v>
       </c>
       <c r="B7">
         <v>85287</v>
@@ -1725,9 +3582,10 @@
         <v>7.2648821039548811E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
-        <v>41685.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41686</v>
       </c>
       <c r="B8">
         <v>92645</v>
@@ -1746,9 +3604,10 @@
         <v>7.8946516271790168E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
-        <v>41692.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41693</v>
       </c>
       <c r="B9">
         <v>91381</v>
@@ -1767,9 +3626,10 @@
         <v>8.9416837198104643E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
-        <v>41699.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41700</v>
       </c>
       <c r="B10">
         <v>89866</v>
@@ -1788,9 +3648,10 @@
         <v>8.366901831615961E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
-        <v>41706.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41707</v>
       </c>
       <c r="B11">
         <v>90660</v>
@@ -1809,9 +3670,10 @@
         <v>8.3675270240458857E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
-        <v>41713.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41714</v>
       </c>
       <c r="B12">
         <v>87847</v>
@@ -1830,9 +3692,10 @@
         <v>8.9041173859095935E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
-        <v>41720.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41721</v>
       </c>
       <c r="B13">
         <v>91209</v>
@@ -1851,9 +3714,10 @@
         <v>8.0978850771305469E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
-        <v>41727.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41728</v>
       </c>
       <c r="B14">
         <v>98857</v>
@@ -1872,9 +3736,10 @@
         <v>9.0089725563187228E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
-        <v>41734.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41735</v>
       </c>
       <c r="B15">
         <v>93279</v>
@@ -1893,9 +3758,10 @@
         <v>9.1799869209575571E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
-        <v>41741.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41742</v>
       </c>
       <c r="B16">
         <v>214835</v>
@@ -1916,7 +3782,8 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
-        <v>41748.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41749</v>
       </c>
       <c r="B17">
         <v>259928</v>
@@ -1937,7 +3804,8 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
-        <v>41755.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41756</v>
       </c>
       <c r="B18">
         <v>230718</v>
@@ -1958,7 +3826,8 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
-        <v>41762.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41763</v>
       </c>
       <c r="B19">
         <v>231385</v>
@@ -1979,7 +3848,8 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
-        <v>41769.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41770</v>
       </c>
       <c r="B20">
         <v>251446</v>
@@ -2000,7 +3870,8 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
-        <v>41776.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41777</v>
       </c>
       <c r="B21">
         <v>276450</v>
@@ -2021,7 +3892,8 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
-        <v>41783.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41784</v>
       </c>
       <c r="B22">
         <v>277902</v>
@@ -2042,7 +3914,8 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
-        <v>41790.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41791</v>
       </c>
       <c r="B23">
         <v>295452</v>
@@ -2063,7 +3936,8 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
-        <v>41797.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41798</v>
       </c>
       <c r="B24">
         <v>309692</v>
@@ -2084,7 +3958,8 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
-        <v>41804.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41805</v>
       </c>
       <c r="B25">
         <v>312461</v>
@@ -2105,7 +3980,8 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
-        <v>41811.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41812</v>
       </c>
       <c r="B26">
         <v>292454</v>
@@ -2126,7 +4002,8 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
-        <v>41818.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41819</v>
       </c>
       <c r="B27">
         <v>306989</v>
@@ -2147,7 +4024,8 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
-        <v>41825.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41826</v>
       </c>
       <c r="B28">
         <v>309321</v>
@@ -2168,7 +4046,8 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
-        <v>41832.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41833</v>
       </c>
       <c r="B29">
         <v>315824</v>
@@ -2189,7 +4068,8 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
-        <v>41839.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41840</v>
       </c>
       <c r="B30">
         <v>304768</v>
@@ -2210,7 +4090,8 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
-        <v>41846.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41847</v>
       </c>
       <c r="B31">
         <v>319995</v>
@@ -2231,7 +4112,8 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
-        <v>41853.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41854</v>
       </c>
       <c r="B32">
         <v>334169</v>
@@ -2252,7 +4134,8 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
-        <v>41860.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41861</v>
       </c>
       <c r="B33">
         <v>281297</v>
@@ -2273,7 +4156,8 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
-        <v>41867.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41868</v>
       </c>
       <c r="B34">
         <v>276196</v>
@@ -2294,7 +4178,8 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
-        <v>41874.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41875</v>
       </c>
       <c r="B35">
         <v>265593</v>
@@ -2315,7 +4200,8 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
-        <v>41881.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41882</v>
       </c>
       <c r="B36">
         <v>255953</v>
@@ -2336,7 +4222,8 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
-        <v>41888.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41889</v>
       </c>
       <c r="B37">
         <v>228440</v>
@@ -2357,7 +4244,8 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
-        <v>41895.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41896</v>
       </c>
       <c r="B38">
         <v>202398</v>
@@ -2378,7 +4266,8 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
-        <v>41902.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41903</v>
       </c>
       <c r="B39">
         <v>176247</v>
@@ -2399,7 +4288,8 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
-        <v>41909.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41910</v>
       </c>
       <c r="B40">
         <v>164752</v>
@@ -2420,7 +4310,8 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
-        <v>41916.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41917</v>
       </c>
       <c r="B41">
         <v>175088</v>
@@ -2441,7 +4332,8 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
-        <v>41923.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41924</v>
       </c>
       <c r="B42">
         <v>175610</v>
@@ -2462,7 +4354,8 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
-        <v>41930.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41931</v>
       </c>
       <c r="B43">
         <v>146095</v>
@@ -2483,7 +4376,8 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
-        <v>41937.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41938</v>
       </c>
       <c r="B44">
         <v>135515</v>
@@ -2504,7 +4398,8 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
-        <v>41944.833333333336</v>
+        <f t="shared" si="1"/>
+        <v>41945</v>
       </c>
       <c r="B45">
         <v>144139</v>
@@ -2525,7 +4420,8 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
-        <v>41951.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41952</v>
       </c>
       <c r="B46">
         <v>129788</v>
@@ -2546,7 +4442,8 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
-        <v>41958.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41959</v>
       </c>
       <c r="B47">
         <v>43840</v>
@@ -2567,7 +4464,8 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
-        <v>41965.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41966</v>
       </c>
       <c r="B48">
         <v>149012</v>
@@ -2588,7 +4486,8 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
-        <v>41972.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41973</v>
       </c>
       <c r="B49">
         <v>143862</v>
@@ -2609,7 +4508,8 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
-        <v>41979.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41980</v>
       </c>
       <c r="B50">
         <v>129754</v>
@@ -2630,7 +4530,8 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
-        <v>41986.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41987</v>
       </c>
       <c r="B51">
         <v>139904</v>
@@ -2651,7 +4552,8 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
-        <v>41993.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>41994</v>
       </c>
       <c r="B52">
         <v>147978</v>
@@ -2672,7 +4574,8 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
-        <v>42000.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>42001</v>
       </c>
       <c r="B53">
         <v>144539</v>
@@ -2693,7 +4596,8 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
-        <v>42007.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>42008</v>
       </c>
       <c r="B54">
         <v>139955</v>
@@ -2714,7 +4618,8 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
-        <v>42014.791666666664</v>
+        <f t="shared" si="1"/>
+        <v>42015</v>
       </c>
       <c r="B55">
         <v>135035</v>

</xml_diff>